<commit_message>
Fixed data for exciter saturation parameters.
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_vsc.xlsx
+++ b/andes/cases/kundur/kundur_vsc.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630D1E25-E740-5A44-BB29-533B6CFD1E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="20220" yWindow="4720" windowWidth="24900" windowHeight="16480" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="1" r:id="rId1"/>
@@ -22,7 +28,7 @@
     <sheet name="R" sheetId="13" r:id="rId13"/>
     <sheet name="VSCShunt" sheetId="14" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -476,8 +482,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,6 +546,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -586,7 +600,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -618,9 +632,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -652,6 +684,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -827,17 +877,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -860,7 +910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -883,7 +933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -912,17 +962,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -984,7 +1034,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1019,7 +1069,7 @@
         <v>1.246</v>
       </c>
       <c r="L2">
-        <v>0.07539999999999999</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="M2">
         <v>20</v>
@@ -1040,13 +1090,13 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1081,7 +1131,7 @@
         <v>1.246</v>
       </c>
       <c r="L3">
-        <v>0.07539999999999999</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="M3">
         <v>20</v>
@@ -1102,13 +1152,13 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1143,7 +1193,7 @@
         <v>1.246</v>
       </c>
       <c r="L4">
-        <v>0.07539999999999999</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="M4">
         <v>20</v>
@@ -1164,13 +1214,13 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1205,7 +1255,7 @@
         <v>1.246</v>
       </c>
       <c r="L5">
-        <v>0.07539999999999999</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="M5">
         <v>20</v>
@@ -1226,10 +1276,10 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1238,7 +1288,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1246,9 +1296,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1286,7 +1336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1315,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1344,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1379,7 +1429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1387,9 +1437,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1409,7 +1459,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1435,7 +1485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1443,9 +1493,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1477,7 +1527,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1515,7 +1565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1523,9 +1573,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1611,7 +1661,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1646,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="M2">
         <v>0.06</v>
@@ -1697,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1732,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="M3">
         <v>0.06</v>
@@ -1789,7 +1839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1797,9 +1847,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1843,7 +1893,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1860,7 +1910,7 @@
         <v>20</v>
       </c>
       <c r="F2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G2">
         <v>0.9</v>
@@ -1869,7 +1919,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0.5702549171626017</v>
+        <v>0.57025491716260168</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -1887,7 +1937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1904,7 +1954,7 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G3">
         <v>0.9</v>
@@ -1913,7 +1963,7 @@
         <v>0.99761</v>
       </c>
       <c r="I3">
-        <v>0.3687461830443478</v>
+        <v>0.36874618304434781</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1931,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1948,16 +1998,16 @@
         <v>20</v>
       </c>
       <c r="F4">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G4">
         <v>0.9</v>
       </c>
       <c r="H4">
-        <v>0.96263</v>
+        <v>0.96262999999999999</v>
       </c>
       <c r="I4">
-        <v>0.1853173146475028</v>
+        <v>0.18531731464750281</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1975,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1992,16 +2042,16 @@
         <v>20</v>
       </c>
       <c r="F5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G5">
         <v>0.9</v>
       </c>
       <c r="H5">
-        <v>0.81691</v>
+        <v>0.81691000000000003</v>
       </c>
       <c r="I5">
-        <v>0.462358662804314</v>
+        <v>0.46235866280431398</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -2019,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2036,16 +2086,16 @@
         <v>230</v>
       </c>
       <c r="F6">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G6">
         <v>0.9</v>
       </c>
       <c r="H6">
-        <v>0.97928</v>
+        <v>0.97928000000000004</v>
       </c>
       <c r="I6">
-        <v>0.4802029090767038</v>
+        <v>0.48020290907670382</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -2063,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2080,16 +2130,16 @@
         <v>230</v>
       </c>
       <c r="F7">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G7">
         <v>0.9</v>
       </c>
       <c r="H7">
-        <v>0.95796</v>
+        <v>0.95796000000000003</v>
       </c>
       <c r="I7">
-        <v>0.2838865294831329</v>
+        <v>0.28388652948313292</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -2107,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2124,16 +2174,16 @@
         <v>230</v>
       </c>
       <c r="F8">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G8">
         <v>0.9</v>
       </c>
       <c r="H8">
-        <v>0.9362</v>
+        <v>0.93620000000000003</v>
       </c>
       <c r="I8">
-        <v>0.1269011445832536</v>
+        <v>0.12690114458325361</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -2151,7 +2201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2168,16 +2218,16 @@
         <v>230</v>
       </c>
       <c r="F9">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G9">
         <v>0.9</v>
       </c>
       <c r="H9">
-        <v>0.87904</v>
+        <v>0.87904000000000004</v>
       </c>
       <c r="I9">
-        <v>-0.0805923235400888</v>
+        <v>-8.0592323540088801E-2</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -2195,7 +2245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2212,7 +2262,7 @@
         <v>230</v>
       </c>
       <c r="F10">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G10">
         <v>0.9</v>
@@ -2221,7 +2271,7 @@
         <v>0.89054</v>
       </c>
       <c r="I10">
-        <v>0.09361771574772226</v>
+        <v>9.3617715747722263E-2</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -2239,7 +2289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2256,16 +2306,16 @@
         <v>230</v>
       </c>
       <c r="F11">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G11">
         <v>0.9</v>
       </c>
       <c r="H11">
-        <v>0.82958</v>
+        <v>0.82957999999999998</v>
       </c>
       <c r="I11">
-        <v>0.3366007088811167</v>
+        <v>0.33660070888111671</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -2289,7 +2339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2297,9 +2347,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2334,7 +2384,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2354,10 +2404,10 @@
         <v>11.59</v>
       </c>
       <c r="H2">
-        <v>-0.735</v>
+        <v>-0.73499999999999999</v>
       </c>
       <c r="I2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J2">
         <v>0.9</v>
@@ -2366,7 +2416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2386,10 +2436,10 @@
         <v>15.75</v>
       </c>
       <c r="H3">
-        <v>-0.899</v>
+        <v>-0.89900000000000002</v>
       </c>
       <c r="I3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J3">
         <v>0.9</v>
@@ -2404,7 +2454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2412,9 +2462,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2473,7 +2523,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2526,7 +2576,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2579,7 +2629,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2638,7 +2688,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2646,9 +2696,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2710,7 +2760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2730,10 +2780,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>7.45861</v>
+        <v>7.4586100000000002</v>
       </c>
       <c r="J2">
-        <v>1.43612</v>
+        <v>1.4361200000000001</v>
       </c>
       <c r="K2">
         <v>9</v>
@@ -2763,7 +2813,7 @@
         <v>0.25</v>
       </c>
       <c r="T2">
-        <v>0.5702549171626017</v>
+        <v>0.57025491716260168</v>
       </c>
     </row>
   </sheetData>
@@ -2772,7 +2822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2780,9 +2830,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2856,7 +2906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2885,13 +2935,13 @@
         <v>230</v>
       </c>
       <c r="K2">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="L2">
         <v>0.05</v>
       </c>
       <c r="M2">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -2918,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2947,13 +2997,13 @@
         <v>230</v>
       </c>
       <c r="K3">
-        <v>0.00501</v>
+        <v>5.0099999999999997E-3</v>
       </c>
       <c r="L3">
-        <v>0.05001</v>
+        <v>5.0009999999999999E-2</v>
       </c>
       <c r="M3">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -2980,7 +3030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3009,7 +3059,7 @@
         <v>230</v>
       </c>
       <c r="K4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="L4">
         <v>0.02</v>
@@ -3042,7 +3092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3071,10 +3121,10 @@
         <v>230</v>
       </c>
       <c r="K5">
-        <v>0.00201</v>
+        <v>2.0100000000000001E-3</v>
       </c>
       <c r="L5">
-        <v>0.02001</v>
+        <v>2.001E-2</v>
       </c>
       <c r="M5">
         <v>0.03</v>
@@ -3104,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3133,10 +3183,10 @@
         <v>230</v>
       </c>
       <c r="K6">
-        <v>0.02201</v>
+        <v>2.2009999999999998E-2</v>
       </c>
       <c r="L6">
-        <v>0.22001</v>
+        <v>0.22001000000000001</v>
       </c>
       <c r="M6">
         <v>0.33</v>
@@ -3166,7 +3216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3195,10 +3245,10 @@
         <v>230</v>
       </c>
       <c r="K7">
-        <v>0.02202</v>
+        <v>2.2020000000000001E-2</v>
       </c>
       <c r="L7">
-        <v>0.22002</v>
+        <v>0.22001999999999999</v>
       </c>
       <c r="M7">
         <v>0.33</v>
@@ -3228,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3257,7 +3307,7 @@
         <v>230</v>
       </c>
       <c r="K8">
-        <v>0.022</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="L8">
         <v>0.22</v>
@@ -3290,7 +3340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3319,7 +3369,7 @@
         <v>230</v>
       </c>
       <c r="K9">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="L9">
         <v>0.02</v>
@@ -3352,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3381,10 +3431,10 @@
         <v>230</v>
       </c>
       <c r="K10">
-        <v>0.00201</v>
+        <v>2.0100000000000001E-3</v>
       </c>
       <c r="L10">
-        <v>0.02001</v>
+        <v>2.001E-2</v>
       </c>
       <c r="M10">
         <v>0.03</v>
@@ -3414,7 +3464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3443,13 +3493,13 @@
         <v>230</v>
       </c>
       <c r="K11">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="L11">
         <v>0.05</v>
       </c>
       <c r="M11">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -3476,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3505,13 +3555,13 @@
         <v>230</v>
       </c>
       <c r="K12">
-        <v>0.00501</v>
+        <v>5.0099999999999997E-3</v>
       </c>
       <c r="L12">
-        <v>0.05001</v>
+        <v>5.0009999999999999E-2</v>
       </c>
       <c r="M12">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -3538,7 +3588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3567,10 +3617,10 @@
         <v>230</v>
       </c>
       <c r="K13">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L13">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -3600,7 +3650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3629,10 +3679,10 @@
         <v>230</v>
       </c>
       <c r="K14">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L14">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -3662,7 +3712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3691,10 +3741,10 @@
         <v>230</v>
       </c>
       <c r="K15">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L15">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -3724,7 +3774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3753,10 +3803,10 @@
         <v>230</v>
       </c>
       <c r="K16">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L16">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -3792,7 +3842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3800,9 +3850,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3816,7 +3866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3830,7 +3880,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3850,7 +3900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3858,9 +3908,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3946,7 +3996,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4011,7 +4061,7 @@
         <v>0.25</v>
       </c>
       <c r="W2">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X2">
         <v>0.25</v>
@@ -4029,7 +4079,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4094,7 +4144,7 @@
         <v>0.25</v>
       </c>
       <c r="W3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X3">
         <v>0.25</v>
@@ -4112,7 +4162,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4177,7 +4227,7 @@
         <v>0.25</v>
       </c>
       <c r="W4">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X4">
         <v>0.25</v>
@@ -4195,7 +4245,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4260,7 +4310,7 @@
         <v>0.25</v>
       </c>
       <c r="W5">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X5">
         <v>0.25</v>
@@ -4284,7 +4334,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4292,9 +4342,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4338,7 +4388,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4379,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4420,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4461,7 +4511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>

</xml_diff>